<commit_message>
add country profile links to schuldenreport_vorlage.xlsx and sr20_erlassjahr.RData
</commit_message>
<xml_diff>
--- a/schuldenreport_vorlage.xlsx
+++ b/schuldenreport_vorlage.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P197"/>
+  <dimension ref="A1:W197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -385,57 +385,92 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>extraktivismus</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>fragilitaet</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>problematische_schuldenstruktur</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>vulnerabilitaet_naturkatastrophen</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>zahlungssituation</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>income</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>oeffentliche_schulden_bip</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>trend_oe_schulden_bip</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>oeffentliche_schulden_staatseinnahmen</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>trend_oe_schulden_staat</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>auslandsschulden_bip</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>trend_ausl_bip</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>auslandsschuldenstand_exporteinnahmen</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>trend_aus_schuldenstand_export</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>auslandsschuldendienst_exporteinnahmen</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>trend_ausl_schuldendienst_export</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>iwf_einschaetzung</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>extraktivismus</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>fragilitaet</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>problematische_schuldenstruktur</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>vulnerabilitaet_naturkatastrophen</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>zahlungssituation</t>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>link</t>
         </is>
       </c>
     </row>
@@ -479,6 +514,16 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/afghanistan/</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -502,6 +547,16 @@
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/angola/</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -525,6 +580,16 @@
       <c r="E5">
         <v>0</v>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/albanien/</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -566,6 +631,16 @@
       <c r="E7">
         <v>0</v>
       </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/argentinien/</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -589,6 +664,16 @@
       <c r="E8">
         <v>0</v>
       </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/armenien/</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -612,6 +697,16 @@
       <c r="E9">
         <v>0</v>
       </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/antigua-barbuda/</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -689,6 +784,16 @@
       <c r="E13">
         <v>0</v>
       </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/burundi/</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -730,6 +835,16 @@
       <c r="E15">
         <v>0</v>
       </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/benin/</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -753,6 +868,16 @@
       <c r="E16">
         <v>0</v>
       </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/burkina-faso/</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -776,6 +901,16 @@
       <c r="E17">
         <v>0</v>
       </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/bangladesch/</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -817,6 +952,16 @@
       <c r="E19">
         <v>0</v>
       </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/bahrain/</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -840,6 +985,16 @@
       <c r="E20">
         <v>0</v>
       </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/bahamas/</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -863,6 +1018,16 @@
       <c r="E21">
         <v>0</v>
       </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/bosnien-herzigowina/</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -886,6 +1051,16 @@
       <c r="E22">
         <v>0</v>
       </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/weissrussland/</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -909,6 +1084,16 @@
       <c r="E23">
         <v>0</v>
       </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/belize/</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -932,6 +1117,16 @@
       <c r="E24">
         <v>0</v>
       </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/bolivien/</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -955,6 +1150,16 @@
       <c r="E25">
         <v>0</v>
       </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/brasilien/</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -978,6 +1183,16 @@
       <c r="E26">
         <v>0</v>
       </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/barbados/</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1019,6 +1234,16 @@
       <c r="E28">
         <v>0</v>
       </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/bhutan/</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1037,6 +1262,11 @@
       <c r="E29">
         <v>0</v>
       </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/aserbaidschan/</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1060,6 +1290,16 @@
       <c r="E30">
         <v>0</v>
       </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/zentralafrikanische-republik/</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1137,6 +1377,16 @@
       <c r="E34">
         <v>0</v>
       </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/china/</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1160,6 +1410,16 @@
       <c r="E35">
         <v>0</v>
       </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/elfenbeinkueste/</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1183,6 +1443,16 @@
       <c r="E36">
         <v>0</v>
       </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/kamerun/</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1206,6 +1476,16 @@
       <c r="E37">
         <v>0</v>
       </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/kongo-d-r/</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1229,6 +1509,16 @@
       <c r="E38">
         <v>0</v>
       </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/republik-kongo/</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1252,6 +1542,16 @@
       <c r="E39">
         <v>0</v>
       </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/kolumbien/</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1275,6 +1575,16 @@
       <c r="E40">
         <v>0</v>
       </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/komoren/</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1298,6 +1608,16 @@
       <c r="E41">
         <v>0</v>
       </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/cabo-verde/</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1321,6 +1641,16 @@
       <c r="E42">
         <v>0</v>
       </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/costa-rica/</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1416,6 +1746,16 @@
       <c r="E47">
         <v>0</v>
       </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/dschibuti/</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1439,6 +1779,16 @@
       <c r="E48">
         <v>0</v>
       </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/dominica/</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1480,6 +1830,16 @@
       <c r="E50">
         <v>0</v>
       </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W50" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/dominikanische-republik/</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1498,6 +1858,11 @@
       <c r="E51">
         <v>0</v>
       </c>
+      <c r="W51" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/algerien/</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1521,6 +1886,16 @@
       <c r="E52">
         <v>0</v>
       </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/ecuador/</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1544,6 +1919,16 @@
       <c r="E53">
         <v>0</v>
       </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/aegypten/</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1567,6 +1952,16 @@
       <c r="E54">
         <v>0</v>
       </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W54" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/eritrea/</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1626,6 +2021,16 @@
       <c r="E57">
         <v>0</v>
       </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W57" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/aethiopien/</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1662,6 +2067,11 @@
       <c r="E59">
         <v>0</v>
       </c>
+      <c r="W59" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/fidschi/</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1703,6 +2113,16 @@
       <c r="E61">
         <v>0</v>
       </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W61" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/mikronesien/</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1726,6 +2146,16 @@
       <c r="E62">
         <v>0</v>
       </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W62" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/gabun/</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1767,6 +2197,16 @@
       <c r="E64">
         <v>0</v>
       </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/georgien/</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1790,6 +2230,16 @@
       <c r="E65">
         <v>0</v>
       </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W65" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/ghana/</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1813,6 +2263,16 @@
       <c r="E66">
         <v>0</v>
       </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W66" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/guinea/</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1836,6 +2296,16 @@
       <c r="E67">
         <v>0</v>
       </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W67" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/gambia/</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1859,6 +2329,16 @@
       <c r="E68">
         <v>0</v>
       </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W68" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/guinea-bissau/</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1877,6 +2357,11 @@
       <c r="E69">
         <v>0</v>
       </c>
+      <c r="W69" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/aequatorialguinea/</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1918,6 +2403,16 @@
       <c r="E71">
         <v>0</v>
       </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W71" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/grenada/</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1941,6 +2436,16 @@
       <c r="E72">
         <v>0</v>
       </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W72" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/guatemala/</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1964,6 +2469,16 @@
       <c r="E73">
         <v>0</v>
       </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W73" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/guyana/</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2005,6 +2520,16 @@
       <c r="E75">
         <v>0</v>
       </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W75" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/honduras/</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2046,6 +2571,16 @@
       <c r="E77">
         <v>0</v>
       </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W77" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/haiti/</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2087,6 +2622,16 @@
       <c r="E79">
         <v>0</v>
       </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W79" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/indonesien/</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2110,6 +2655,16 @@
       <c r="E80">
         <v>0</v>
       </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W80" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/indien/</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2151,6 +2706,16 @@
       <c r="E82">
         <v>0</v>
       </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W82" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/iran/</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2169,6 +2734,11 @@
       <c r="E83">
         <v>0</v>
       </c>
+      <c r="W83" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/irak/</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2246,6 +2816,16 @@
       <c r="E87">
         <v>0</v>
       </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W87" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/jamaika/</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2269,6 +2849,16 @@
       <c r="E88">
         <v>0</v>
       </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W88" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/jordanien/</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2310,6 +2900,16 @@
       <c r="E90">
         <v>0</v>
       </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W90" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/kasachstan/</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2333,6 +2933,16 @@
       <c r="E91">
         <v>0</v>
       </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W91" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/kenia/</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2356,6 +2966,16 @@
       <c r="E92">
         <v>0</v>
       </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W92" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/kirgisistan/</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2379,6 +2999,16 @@
       <c r="E93">
         <v>0</v>
       </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W93" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/kambodscha/</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2402,6 +3032,16 @@
       <c r="E94">
         <v>0</v>
       </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W94" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/kiribati/</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2425,6 +3065,16 @@
       <c r="E95">
         <v>0</v>
       </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="W95" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/st.-kitts-nevis/</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2484,6 +3134,16 @@
       <c r="E98">
         <v>0</v>
       </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W98" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/laos/</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2507,6 +3167,16 @@
       <c r="E99">
         <v>0</v>
       </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W99" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/libanon/</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2530,6 +3200,16 @@
       <c r="E100">
         <v>0</v>
       </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W100" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/liberia/</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2571,6 +3251,16 @@
       <c r="E102">
         <v>0</v>
       </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W102" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/st-lucia/</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -2594,6 +3284,16 @@
       <c r="E103">
         <v>0</v>
       </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W103" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/sri-lanka/</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -2612,6 +3312,11 @@
       <c r="E104">
         <v>0</v>
       </c>
+      <c r="W104" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/lesotho/</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2707,6 +3412,16 @@
       <c r="E109">
         <v>0</v>
       </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W109" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/marokko/</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2730,6 +3445,16 @@
       <c r="E110">
         <v>0</v>
       </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W110" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/moldau/</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2753,6 +3478,16 @@
       <c r="E111">
         <v>0</v>
       </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W111" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/madagaskar/</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2776,6 +3511,16 @@
       <c r="E112">
         <v>0</v>
       </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W112" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/malediven/</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2799,6 +3544,16 @@
       <c r="E113">
         <v>0</v>
       </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W113" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/mexiko/</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2822,6 +3577,16 @@
       <c r="E114">
         <v>0</v>
       </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W114" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/marshallinseln/</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2845,6 +3610,16 @@
       <c r="E115">
         <v>0</v>
       </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W115" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/mazedonien/</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2868,6 +3643,16 @@
       <c r="E116">
         <v>0</v>
       </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W116" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/mali/</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2909,6 +3694,16 @@
       <c r="E118">
         <v>0</v>
       </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W118" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/myanmar/</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2932,6 +3727,16 @@
       <c r="E119">
         <v>0</v>
       </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W119" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/montenegro/</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2955,6 +3760,16 @@
       <c r="E120">
         <v>0</v>
       </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W120" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/mongolei/</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2978,6 +3793,16 @@
       <c r="E121">
         <v>0</v>
       </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W121" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/mosambik/</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3001,6 +3826,16 @@
       <c r="E122">
         <v>0</v>
       </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W122" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/mauretanien/</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3024,6 +3859,16 @@
       <c r="E123">
         <v>0</v>
       </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W123" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/mauritius/</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -3047,6 +3892,16 @@
       <c r="E124">
         <v>0</v>
       </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W124" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/malawi/</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -3070,6 +3925,16 @@
       <c r="E125">
         <v>0</v>
       </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W125" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/malaysia/</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3093,6 +3958,16 @@
       <c r="E126">
         <v>0</v>
       </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W126" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/namibia/</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -3116,6 +3991,16 @@
       <c r="E127">
         <v>0</v>
       </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W127" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/niger/</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -3139,6 +4024,16 @@
       <c r="E128">
         <v>0</v>
       </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W128" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/nigeria/</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3162,6 +4057,16 @@
       <c r="E129">
         <v>0</v>
       </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W129" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/nicaragua/</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3216,6 +4121,11 @@
       <c r="E132">
         <v>0</v>
       </c>
+      <c r="W132" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/nepal/</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -3239,6 +4149,11 @@
       <c r="E133">
         <v>0</v>
       </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -3280,6 +4195,11 @@
       <c r="E135">
         <v>0</v>
       </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -3303,6 +4223,16 @@
       <c r="E136">
         <v>0</v>
       </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W136" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/pakistan/</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -3326,6 +4256,16 @@
       <c r="E137">
         <v>0</v>
       </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="W137" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/panama/</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -3349,6 +4289,16 @@
       <c r="E138">
         <v>0</v>
       </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W138" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/peru/</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -3367,6 +4317,11 @@
       <c r="E139">
         <v>0</v>
       </c>
+      <c r="W139" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/philippinen/</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -3408,6 +4363,16 @@
       <c r="E141">
         <v>0</v>
       </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W141" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/papua-neuguinea/</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -3503,6 +4468,16 @@
       <c r="E146">
         <v>0</v>
       </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W146" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/paraguay/</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -3539,6 +4514,11 @@
       <c r="E148">
         <v>0</v>
       </c>
+      <c r="W148" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/kosovo/</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -3598,6 +4578,16 @@
       <c r="E151">
         <v>0</v>
       </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W151" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/ruanda/</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -3639,6 +4629,16 @@
       <c r="E153">
         <v>0</v>
       </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W153" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/sudan/</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -3662,6 +4662,16 @@
       <c r="E154">
         <v>0</v>
       </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W154" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/senegal/</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -3685,6 +4695,11 @@
       <c r="E155">
         <v>0</v>
       </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -3703,6 +4718,11 @@
       <c r="E156">
         <v>0</v>
       </c>
+      <c r="W156" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/salomonen/</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -3726,6 +4746,16 @@
       <c r="E157">
         <v>0</v>
       </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W157" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/sierra-leone/</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -3749,6 +4779,16 @@
       <c r="E158">
         <v>0</v>
       </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W158" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/el-salvador/</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -3785,6 +4825,11 @@
       <c r="E160">
         <v>1</v>
       </c>
+      <c r="W160" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/somalia/</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -3808,6 +4853,16 @@
       <c r="E161">
         <v>0</v>
       </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W161" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/serbien/</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -3831,6 +4886,16 @@
       <c r="E162">
         <v>0</v>
       </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W162" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/suedsudan/</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -3854,6 +4919,16 @@
       <c r="E163">
         <v>0</v>
       </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W163" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/sao-tome-principe/</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -3877,6 +4952,16 @@
       <c r="E164">
         <v>0</v>
       </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W164" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/surinam/</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -3949,6 +5034,11 @@
       <c r="E168">
         <v>0</v>
       </c>
+      <c r="W168" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/swasiland/</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -3972,6 +5062,16 @@
       <c r="E169">
         <v>0</v>
       </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="W169" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/seychellen/</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -3990,6 +5090,11 @@
       <c r="E170">
         <v>1</v>
       </c>
+      <c r="W170" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/syrien/</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -4013,6 +5118,16 @@
       <c r="E171">
         <v>0</v>
       </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W171" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/tschad/</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -4036,6 +5151,16 @@
       <c r="E172">
         <v>0</v>
       </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W172" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/togo/</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -4054,6 +5179,11 @@
       <c r="E173">
         <v>0</v>
       </c>
+      <c r="W173" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/thailand/</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -4077,6 +5207,16 @@
       <c r="E174">
         <v>0</v>
       </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W174" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/tadschikistan/</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -4100,6 +5240,11 @@
       <c r="E175">
         <v>0</v>
       </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -4118,6 +5263,11 @@
       <c r="E176">
         <v>0</v>
       </c>
+      <c r="W176" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/ost-timor/</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -4141,6 +5291,16 @@
       <c r="E177">
         <v>0</v>
       </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W177" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/tonga/</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -4159,6 +5319,11 @@
       <c r="E178">
         <v>0</v>
       </c>
+      <c r="W178" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/trinidad-tobago/</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -4182,6 +5347,16 @@
       <c r="E179">
         <v>0</v>
       </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W179" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/tunesien/</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -4205,6 +5380,16 @@
       <c r="E180">
         <v>0</v>
       </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W180" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/tuerkei/</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -4228,6 +5413,16 @@
       <c r="E181">
         <v>0</v>
       </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W181" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/tuvalu/</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -4251,6 +5446,16 @@
       <c r="E182">
         <v>0</v>
       </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="W182" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/taiwan/</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -4274,6 +5479,16 @@
       <c r="E183">
         <v>0</v>
       </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W183" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/tansania/</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -4297,6 +5512,16 @@
       <c r="E184">
         <v>0</v>
       </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="W184" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/uganda/</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -4320,6 +5545,16 @@
       <c r="E185">
         <v>0</v>
       </c>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W185" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/ukraine/</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -4343,6 +5578,16 @@
       <c r="E186">
         <v>0</v>
       </c>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="W186" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/uruguay/</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -4379,6 +5624,11 @@
       <c r="E188">
         <v>0</v>
       </c>
+      <c r="W188" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/usbekistan/</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -4402,6 +5652,16 @@
       <c r="E189">
         <v>0</v>
       </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W189" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/st-vincent/</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -4425,6 +5685,16 @@
       <c r="E190">
         <v>0</v>
       </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W190" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/venezuela/</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -4448,6 +5718,16 @@
       <c r="E191">
         <v>0</v>
       </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W191" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/vietnam/</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -4471,6 +5751,16 @@
       <c r="E192">
         <v>0</v>
       </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W192" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/vanuatu/</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -4494,6 +5784,16 @@
       <c r="E193">
         <v>0</v>
       </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W193" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/samoa/</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -4517,6 +5817,16 @@
       <c r="E194">
         <v>0</v>
       </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W194" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/jemen/</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -4540,6 +5850,16 @@
       <c r="E195">
         <v>0</v>
       </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>um</t>
+        </is>
+      </c>
+      <c r="W195" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/suedafrika/</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -4563,6 +5883,16 @@
       <c r="E196">
         <v>0</v>
       </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W196" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/sambia/</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -4585,6 +5915,16 @@
       </c>
       <c r="E197">
         <v>0</v>
+      </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="W197" t="inlineStr">
+        <is>
+          <t>https://erlassjahr.de/laenderinfos/simbabwe/</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>